<commit_message>
file changed after re run of scraper.py
</commit_message>
<xml_diff>
--- a/cases.xlsx
+++ b/cases.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Corona cases" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Corona cases" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,60 +424,72 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>80,011,873</t>
+          <t>56,827,972</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>38,532,895</t>
+          <t>80,098,585</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>66,140,595</t>
+          <t>38,549,148</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Africa</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>8,605,714</t>
+          <t>66,352,163</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>Africa</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>8,608,324</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>Oceania</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>323,323</t>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>325,319</t>
         </is>
       </c>
     </row>

</xml_diff>